<commit_message>
working feature. Needs coding improvements.
</commit_message>
<xml_diff>
--- a/listados/pedidos-base.xlsx
+++ b/listados/pedidos-base.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$H$33</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -108,9 +111,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -137,8 +147,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,148 +436,408 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A26"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>